<commit_message>
Added System Properties in pom.xml, implemented parallel testing for data driven tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginData.xlsx
+++ b/src/test/resources/testdata/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Projects\LearningSelenuimV1\data-driven-test-practice\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7C8EAF-446A-4298-BD72-4A08E9FD9CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999876F5-7684-4B89-A930-408FDDC8F278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43CC7555-4A46-49BF-A831-1CED037CF33C}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>